<commit_message>
ECU-9 creado, Modificar informacion basica pacientes
</commit_message>
<xml_diff>
--- a/documentos/CronogramaTSP.xlsx
+++ b/documentos/CronogramaTSP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="460" yWindow="260" windowWidth="25040" windowHeight="14920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>Tarea</t>
   </si>
@@ -114,15 +114,6 @@
     <t>ECU. Modificar historial médico de forma local</t>
   </si>
   <si>
-    <t>ECU. Crear pacientes</t>
-  </si>
-  <si>
-    <t>ECU. Crear propietarios</t>
-  </si>
-  <si>
-    <t>ECU. Crear MVZ's</t>
-  </si>
-  <si>
     <t>ECU. Registrar historial médico desde internet</t>
   </si>
   <si>
@@ -166,6 +157,15 @@
   </si>
   <si>
     <t>Juan Esteban</t>
+  </si>
+  <si>
+    <t>ECU. Registrar pacientes</t>
+  </si>
+  <si>
+    <t>ECU. Registrar propietarios</t>
+  </si>
+  <si>
+    <t>ECU. Registrar MVZ's</t>
   </si>
 </sst>
 </file>
@@ -915,7 +915,7 @@
   <dimension ref="B2:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -951,7 +951,7 @@
         <v>6</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:9">
@@ -971,7 +971,7 @@
         <v>26</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:9">
@@ -991,7 +991,7 @@
         <v>26</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:9">
@@ -1041,7 +1041,7 @@
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:9">
@@ -1077,50 +1077,52 @@
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:9">
-      <c r="B10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="9">
-        <v>2</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9">
-        <v>9</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9">
-        <v>2</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9" t="s">
+      <c r="B10" s="6" t="s">
         <v>46</v>
       </c>
+      <c r="C10" s="7">
+        <v>2</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7">
+        <v>2</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="11" spans="2:9">
-      <c r="B11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="9">
-        <v>2</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9">
-        <v>2</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9" t="s">
-        <v>46</v>
+      <c r="B11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="7">
+        <v>2</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7">
+        <v>2</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="8" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C12" s="9">
         <v>2</v>
@@ -1133,12 +1135,12 @@
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C13" s="7">
         <v>2</v>
@@ -1153,48 +1155,52 @@
         <v>26</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="2:9">
-      <c r="B14" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="9">
-        <v>2</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9">
-        <v>2</v>
-      </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9" t="s">
-        <v>45</v>
+      <c r="B14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="7">
+        <v>2</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7">
+        <v>2</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:9">
-      <c r="B15" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="9">
-        <v>2</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9">
-        <v>2</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9" t="s">
-        <v>45</v>
+      <c r="B15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7">
+        <v>2</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="2:9">
       <c r="B16" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C16" s="9">
         <v>1</v>
@@ -1207,12 +1213,12 @@
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:9">
       <c r="B17" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C17" s="9">
         <v>1</v>
@@ -1225,12 +1231,12 @@
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="2:9">
       <c r="B18" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C18" s="9">
         <v>1</v>
@@ -1243,12 +1249,12 @@
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="2:9">
       <c r="B19" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C19" s="9">
         <v>1</v>
@@ -1264,7 +1270,7 @@
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C20" s="9">
         <v>1</v>
@@ -1280,7 +1286,7 @@
     </row>
     <row r="21" spans="2:9">
       <c r="B21" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C21" s="9">
         <v>1</v>
@@ -1296,7 +1302,7 @@
     </row>
     <row r="22" spans="2:9">
       <c r="B22" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C22" s="9">
         <v>1</v>
@@ -1312,7 +1318,7 @@
     </row>
     <row r="23" spans="2:9">
       <c r="B23" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C23" s="9">
         <v>1</v>
@@ -1328,7 +1334,7 @@
     </row>
     <row r="24" spans="2:9">
       <c r="B24" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C24" s="9">
         <v>1</v>
@@ -1359,7 +1365,7 @@
         <v>26</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="2:9">
@@ -1679,7 +1685,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>